<commit_message>
Model and example updates for Hackathon
</commit_message>
<xml_diff>
--- a/utilities/python/ARS Template.xlsx
+++ b/utilities/python/ARS Template.xlsx
@@ -1,32 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDISC\ars\analysis-results-standard\utilities\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F118979-3AAE-420F-AC63-8BFCC8987E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E6BEA5-5EE3-4600-A2DA-C839503CC8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5610" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
   </bookViews>
   <sheets>
-    <sheet name="ListOfPlannedAnalyses" sheetId="10" r:id="rId1"/>
-    <sheet name="Outputs" sheetId="11" r:id="rId2"/>
-    <sheet name="Displays" sheetId="13" r:id="rId3"/>
-    <sheet name="DataSubsets" sheetId="6" r:id="rId4"/>
-    <sheet name="AnalysisSets" sheetId="1" r:id="rId5"/>
-    <sheet name="AnalysisGroupings" sheetId="2" r:id="rId6"/>
-    <sheet name="Analyses" sheetId="3" r:id="rId7"/>
-    <sheet name="AnalysisMethods" sheetId="4" r:id="rId8"/>
-    <sheet name="AnalysisResults" sheetId="7" r:id="rId9"/>
+    <sheet name="ReportingEvent" sheetId="19" r:id="rId1"/>
+    <sheet name="ReferenceDocuments" sheetId="20" r:id="rId2"/>
+    <sheet name="Categorizations" sheetId="22" r:id="rId3"/>
+    <sheet name="ListOfPlannedAnalyses" sheetId="10" r:id="rId4"/>
+    <sheet name="ListOfPlannedOutputs" sheetId="25" r:id="rId5"/>
+    <sheet name="GlobalDisplaySections" sheetId="35" r:id="rId6"/>
+    <sheet name="Outputs" sheetId="11" r:id="rId7"/>
+    <sheet name="Displays" sheetId="13" r:id="rId8"/>
+    <sheet name="OutputProgrammingCode" sheetId="30" r:id="rId9"/>
+    <sheet name="OutputCodeParameters" sheetId="34" r:id="rId10"/>
+    <sheet name="OutputDocumentRefs" sheetId="31" r:id="rId11"/>
+    <sheet name="DataSubsets" sheetId="6" r:id="rId12"/>
+    <sheet name="AnalysisSets" sheetId="1" r:id="rId13"/>
+    <sheet name="AnalysisGroupings" sheetId="2" r:id="rId14"/>
+    <sheet name="Analyses" sheetId="3" r:id="rId15"/>
+    <sheet name="AnalysisProgrammingCode" sheetId="27" r:id="rId16"/>
+    <sheet name="AnalysisCodeParameters" sheetId="32" r:id="rId17"/>
+    <sheet name="AnalysisDocumentRefs" sheetId="24" r:id="rId18"/>
+    <sheet name="AnalysisMethods" sheetId="4" r:id="rId19"/>
+    <sheet name="AnalysisMethodCodeTemplate" sheetId="23" r:id="rId20"/>
+    <sheet name="AnalysisMethodCodeParameters" sheetId="33" r:id="rId21"/>
+    <sheet name="AnalysisMethodDocumentRefs" sheetId="26" r:id="rId22"/>
+    <sheet name="AnalysisResults" sheetId="7" r:id="rId23"/>
+    <sheet name="TerminologyExtensions" sheetId="21" r:id="rId24"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Analyses!$A$1:$S$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">AnalysisMethods!$A$1:$N$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">AnalysisResults!$A$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Analyses!$A$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AnalysisDocumentRefs!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AnalysisMethods!$A$1:$P$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">AnalysisProgrammingCode!$A$1:$D$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AnalysisResults!$A$1:$U$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">DataSubsets!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Displays!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">OutputDocumentRefs!$A$1:$F$2</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -48,8 +68,99 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Richard</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{44ED35CB-7EEE-4AA9-9B4E-6D9C40C1D98F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Page range n-n (e.g., 6-12), pipe-delmited list of page numbers (e.g., 2|8|12), or pipe-delimited list of named destinations (e.g., Section 2|Section 5).</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Richard</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{74B1AA6A-6FD2-4F74-AD45-9C05B7586857}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Page range n-n (e.g., 6-12), pipe-delmited list of page numbers (e.g., 2|8|12), or pipe-delimited list of named destinations (e.g., Section 2|Section 5).</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Richard</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{BA7913E3-38B4-45EB-9040-CFA873D860CF}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Page range n-n (e.g., 6-12), pipe-delmited list of page numbers (e.g., 2|8|12), or pipe-delimited list of named destinations (e.g., Section 2|Section 5).</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="108">
   <si>
     <t>id</t>
   </si>
@@ -162,9 +273,6 @@
     <t>displaySection_subSection_id</t>
   </si>
   <si>
-    <t>displaySection_subSection_order</t>
-  </si>
-  <si>
     <t>displaySection_subSection_text</t>
   </si>
   <si>
@@ -177,12 +285,6 @@
     <t>analysisSet_label</t>
   </si>
   <si>
-    <t>operation_referencedResultRelationships_description_NUMERATOR</t>
-  </si>
-  <si>
-    <t>operation_referencedResultRelationships_description_DENOMINATOR</t>
-  </si>
-  <si>
     <t>categoryIds</t>
   </si>
   <si>
@@ -213,12 +315,6 @@
     <t>groupingId3</t>
   </si>
   <si>
-    <t>operation_referencedResultRelationships_operationId_NUMERATOR</t>
-  </si>
-  <si>
-    <t>operation_referencedResultRelationships_operationId_DENOMINATOR</t>
-  </si>
-  <si>
     <t>analysisId</t>
   </si>
   <si>
@@ -273,17 +369,128 @@
     <t>resultsByGroup3</t>
   </si>
   <si>
-    <t>operation_referencedResultRelationships_id_NUMERATOR</t>
-  </si>
-  <si>
-    <t>operation_referencedResultRelationships_id_DENOMINATOR</t>
+    <t>location</t>
+  </si>
+  <si>
+    <t>enumeration</t>
+  </si>
+  <si>
+    <t>sponsorTerm_id</t>
+  </si>
+  <si>
+    <t>sponsorTerm_submissionValue</t>
+  </si>
+  <si>
+    <t>sponsorTerm_description</t>
+  </si>
+  <si>
+    <t>reason</t>
+  </si>
+  <si>
+    <t>purpose</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>category_label</t>
+  </si>
+  <si>
+    <t>parent_category_id</t>
+  </si>
+  <si>
+    <t>templateCode</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>analysis_id</t>
+  </si>
+  <si>
+    <t>refDocumentId</t>
+  </si>
+  <si>
+    <t>pageRef_refType</t>
+  </si>
+  <si>
+    <t>pageRef_pages</t>
+  </si>
+  <si>
+    <t>pageRef_label</t>
+  </si>
+  <si>
+    <t>referenceType</t>
+  </si>
+  <si>
+    <t>specifiedAs</t>
+  </si>
+  <si>
+    <t>parameter_name</t>
+  </si>
+  <si>
+    <t>parameter_description</t>
+  </si>
+  <si>
+    <t>parameter_valueSource</t>
+  </si>
+  <si>
+    <t>parameter_value</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>output_id</t>
+  </si>
+  <si>
+    <t>group_level</t>
+  </si>
+  <si>
+    <t>group_compoundExpression_logicalOperator</t>
+  </si>
+  <si>
+    <t>sectionType</t>
+  </si>
+  <si>
+    <t>subSection_id</t>
+  </si>
+  <si>
+    <t>subSection_text</t>
+  </si>
+  <si>
+    <t>displaySection_orderedSubSection_order</t>
+  </si>
+  <si>
+    <t>operation_referencedResultRelationships1_id</t>
+  </si>
+  <si>
+    <t>operation_referencedResultRelationships2_id</t>
+  </si>
+  <si>
+    <t>operation_referencedResultRelationships1_operationId</t>
+  </si>
+  <si>
+    <t>operation_referencedResultRelationships1_referencedOperationRole</t>
+  </si>
+  <si>
+    <t>operation_referencedResultRelationships2_operationId</t>
+  </si>
+  <si>
+    <t>operation_referencedResultRelationships1_description</t>
+  </si>
+  <si>
+    <t>operation_referencedResultRelationships2_referencedOperationRole</t>
+  </si>
+  <si>
+    <t>operation_referencedResultRelationships2_description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +511,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -332,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -342,6 +555,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,65 +872,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04E4817-59BC-4505-A834-22FE96EF578C}">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:E1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5945FE14-B7CD-4113-88D6-525465F971DD}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="85.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1328125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8F6BB7-6ECF-4265-9AA7-E57DC9AB4DDB}">
-  <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="11.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.59765625" customWidth="1"/>
-    <col min="5" max="5" width="35.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.9296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.53125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <col min="3" max="3" width="21.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -722,77 +890,99 @@
         <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB264D80-6970-406C-8A9F-6A5C48FD0FE0}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44891FB9-A2CE-4D40-A988-A4A68CEC1B08}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.796875" customWidth="1"/>
+    <col min="3" max="3" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3266631C-B97C-414A-AC8B-8A56E4E40917}">
-  <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.06640625" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.06640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="27.796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F2" xr:uid="{62E9726D-99E8-44E0-8F39-A719318C5D2B}"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{917ECCE5-EEC8-44A7-B89C-54389CACCCF1}">
+      <formula1>"PhysicalRef,NamedDestination"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{60365E17-9D50-4DB4-A3E8-B6CD667DE4F9}">
+      <formula1>"Documentation,ProgrammingCode"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317E84A7-ED57-45F7-86AC-94BF9578A26E}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I1"/>
@@ -805,7 +995,7 @@
     <col min="2" max="2" width="58.33203125" customWidth="1"/>
     <col min="3" max="3" width="4.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.3984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.53125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="33.1328125" bestFit="1" customWidth="1"/>
@@ -826,7 +1016,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -842,14 +1032,15 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+  <autoFilter ref="A1:I1" xr:uid="{317E84A7-ED57-45F7-86AC-94BF9578A26E}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2057B85-CDD2-49FA-961B-BE66955E248E}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -857,14 +1048,16 @@
   <cols>
     <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -872,18 +1065,24 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -893,10 +1092,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD49E34F-52D6-4F1E-B1C2-4599C0323EA6}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -908,15 +1107,17 @@
     <col min="4" max="4" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.796875" customWidth="1"/>
-    <col min="8" max="8" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.06640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <col min="7" max="7" width="35.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.796875" customWidth="1"/>
+    <col min="11" max="11" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.06640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="46" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -939,21 +1140,33 @@
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A2" t="str">
+        <f t="shared" ref="A2" si="0">IF(K2="ADSL","Subject","Data")</f>
+        <v>Data</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -961,10 +1174,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB53023-B5E5-496E-A786-48C47411B817}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -972,26 +1185,28 @@
   <cols>
     <col min="1" max="1" width="35.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.06640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.46484375" customWidth="1"/>
+    <col min="4" max="4" width="27.73046875" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.53125" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.46484375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.19921875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.86328125" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" customWidth="1"/>
-    <col min="18" max="18" width="28.3984375" customWidth="1"/>
-    <col min="19" max="19" width="16.265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
+    <col min="12" max="12" width="20.53125" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.46484375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.86328125" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" customWidth="1"/>
+    <col min="20" max="20" width="28.3984375" customWidth="1"/>
+    <col min="21" max="21" width="16.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1002,65 +1217,205 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:U1" xr:uid="{4AB53023-B5E5-496E-A786-48C47411B817}"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7330FD-BC60-4063-AD51-1ADCE1E2B7CF}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="34.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D7" s="6"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D7" xr:uid="{1F7330FD-BC60-4063-AD51-1ADCE1E2B7CF}"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C7" xr:uid="{93C20FD9-A520-4F19-96A5-76364810E4EA}">
+      <formula1>"Code,DocumentRef"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCEEFCB-4AF8-4DF4-9DD6-EB21C9658A74}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E9726D-99E8-44E0-8F39-A719318C5D2B}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.796875" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:S1" xr:uid="{4AB53023-B5E5-496E-A786-48C47411B817}"/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{62E9726D-99E8-44E0-8F39-A719318C5D2B}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC97203C-D8B1-4020-B955-08EA542F4944}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1075,11 +1430,15 @@
     <col min="7" max="7" width="23" customWidth="1"/>
     <col min="8" max="8" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="13" width="33.53125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="26.9296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <col min="10" max="10" width="33.53125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.53125" customWidth="1"/>
+    <col min="12" max="13" width="33.53125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.46484375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.73046875" customWidth="1"/>
+    <col min="16" max="17" width="26.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1108,26 +1467,32 @@
         <v>25</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K19">
+        <v>106</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L19">
     <sortCondition ref="A2:A19"/>
     <sortCondition ref="G2:G19"/>
   </sortState>
@@ -1135,10 +1500,171 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63425975-7444-4301-ABB6-796B2115B6F2}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.06640625" customWidth="1"/>
+    <col min="3" max="3" width="43.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5A7EA2-5BB8-48A0-AE19-CC45569B1AA0}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="44.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="D3" s="6"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3" xr:uid="{CC14E9E5-6CF5-4253-837A-778F67077D54}">
+      <formula1>"Code,DocumentRef"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F5578B-A7DE-401B-B867-DFECFDE9AF0A}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26572EB2-03E0-4576-A1FD-245E2B761D42}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.796875" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4" xr:uid="{3A6A89FF-143B-4B65-965D-58F3F87AADFC}">
+      <formula1>"Documentation,ProgrammingCode"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{19E8A5BB-5746-4AF5-8B3B-1D99BD0D0680}">
+      <formula1>"PhysicalRef,NamedDestination"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BB806F-07BC-44FD-839E-73D40D8773BC}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1170,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>26</v>
@@ -1188,40 +1714,40 @@
         <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>27</v>
@@ -1230,10 +1756,509 @@
         <v>28</v>
       </c>
     </row>
-  </sheetData>
-  <autoFilter ref="A1:U1" xr:uid="{41BB806F-07BC-44FD-839E-73D40D8773BC}"/>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="B2" s="3" t="e" cm="1">
+        <f t="array" ref="B2">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A2,""),"")</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D2" s="3" cm="1">
+        <f t="array" ref="D2">_xlfn.UNIQUE(_xlfn._xlws.FILTER(AnalysisMethods!$C$2:$C$19,AnalysisMethods!$A$2:$A$19=AnalysisResults!C2,""))</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" cm="1">
+        <f t="array" ref="F2:F19">_xlfn._xlws.FILTER(AnalysisMethods!$H$2:$H$19,AnalysisMethods!$E$2:$E$19=AnalysisResults!E2,"")</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="3" cm="1">
+        <f t="array" ref="G2:G19">_xlfn._xlws.FILTER(AnalysisMethods!$I$2:$I$19,AnalysisMethods!$E$2:$E$19=AnalysisResults!E2,"")</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="3" t="str" cm="1">
+        <f t="array" ref="J2">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$2,(AnalysisGroupings!$F$2:$F$2=AnalysisResults!I2)*LEN(I2)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="N2" s="3" t="str" cm="1">
+        <f t="array" ref="N2">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$2,(AnalysisGroupings!$F$2:$F$2=AnalysisResults!M2)*LEN(M2)&gt;0,"")</f>
+        <v/>
+      </c>
+      <c r="R2" s="3" t="str" cm="1">
+        <f t="array" ref="R2">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$2,(AnalysisGroupings!$F$2:$F$2=AnalysisResults!Q2)*LEN(Q2)&gt;0,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.45">
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.45">
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.45">
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:U2" xr:uid="{41BB806F-07BC-44FD-839E-73D40D8773BC}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U2">
+    <sortCondition ref="A2"/>
+    <sortCondition ref="C2"/>
+    <sortCondition ref="I2"/>
+  </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C6F21E-B0BD-4A7C-9873-05E64DE79965}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.3984375" customWidth="1"/>
+    <col min="4" max="4" width="52.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A24" xr:uid="{0A7C3BAC-D424-43D3-9B4E-1A4E4E37AE75}">
+      <formula1>"AnalysisReason,AnalysisPurpose,OperationRole,OutputFileType"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A19ABE-6E7C-4DBB-B149-CB6DE6FC596E}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04E4817-59BC-4505-A834-22FE96EF578C}">
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="85.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78005A0C-8AA5-4998-8A42-428CFBB35FD9}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="80.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC151BBF-2F10-45B4-986C-600EDF05B350}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A23" xr:uid="{6F5061BD-D187-4B34-B453-5F022522F44D}">
+      <formula1>"Title,Footnote,Abbreviation,Legend,Rowlabel Header"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B8F6BB7-6ECF-4265-9AA7-E57DC9AB4DDB}">
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="78.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.59765625" customWidth="1"/>
+    <col min="6" max="6" width="35.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3266631C-B97C-414A-AC8B-8A56E4E40917}">
+  <sheetPr codeName="Sheet11"/>
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.06640625" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="27.06640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{3266631C-B97C-414A-AC8B-8A56E4E40917}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF4F43AB-08A9-4D5D-BC36-392099289A62}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="34.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{AFBCF27C-42FB-4934-B668-A0446B0CFA1C}">
+      <formula1>"Code,DocumentRef"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates for ARSP-28, #136, #209, #217, #219, #221, #220
</commit_message>
<xml_diff>
--- a/utilities/python/ARS Template.xlsx
+++ b/utilities/python/ARS Template.xlsx
@@ -1,54 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDISC\ars\analysis-results-standard\utilities\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E6BEA5-5EE3-4600-A2DA-C839503CC8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDB610B-F10C-4889-AC61-E0EF2010FD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
+    <workbookView xWindow="127" yWindow="0" windowWidth="21601" windowHeight="11400" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingEvent" sheetId="19" r:id="rId1"/>
     <sheet name="ReferenceDocuments" sheetId="20" r:id="rId2"/>
     <sheet name="Categorizations" sheetId="22" r:id="rId3"/>
-    <sheet name="ListOfPlannedAnalyses" sheetId="10" r:id="rId4"/>
-    <sheet name="ListOfPlannedOutputs" sheetId="25" r:id="rId5"/>
+    <sheet name="MainListOfContents" sheetId="10" r:id="rId4"/>
+    <sheet name="OtherListsOfContents" sheetId="25" r:id="rId5"/>
     <sheet name="GlobalDisplaySections" sheetId="35" r:id="rId6"/>
     <sheet name="Outputs" sheetId="11" r:id="rId7"/>
-    <sheet name="Displays" sheetId="13" r:id="rId8"/>
-    <sheet name="OutputProgrammingCode" sheetId="30" r:id="rId9"/>
-    <sheet name="OutputCodeParameters" sheetId="34" r:id="rId10"/>
-    <sheet name="OutputDocumentRefs" sheetId="31" r:id="rId11"/>
-    <sheet name="DataSubsets" sheetId="6" r:id="rId12"/>
-    <sheet name="AnalysisSets" sheetId="1" r:id="rId13"/>
-    <sheet name="AnalysisGroupings" sheetId="2" r:id="rId14"/>
-    <sheet name="Analyses" sheetId="3" r:id="rId15"/>
-    <sheet name="AnalysisProgrammingCode" sheetId="27" r:id="rId16"/>
-    <sheet name="AnalysisCodeParameters" sheetId="32" r:id="rId17"/>
-    <sheet name="AnalysisDocumentRefs" sheetId="24" r:id="rId18"/>
-    <sheet name="AnalysisMethods" sheetId="4" r:id="rId19"/>
-    <sheet name="AnalysisMethodCodeTemplate" sheetId="23" r:id="rId20"/>
-    <sheet name="AnalysisMethodCodeParameters" sheetId="33" r:id="rId21"/>
-    <sheet name="AnalysisMethodDocumentRefs" sheetId="26" r:id="rId22"/>
-    <sheet name="AnalysisResults" sheetId="7" r:id="rId23"/>
-    <sheet name="TerminologyExtensions" sheetId="21" r:id="rId24"/>
+    <sheet name="OutputFiles" sheetId="36" r:id="rId8"/>
+    <sheet name="Displays" sheetId="13" r:id="rId9"/>
+    <sheet name="OutputProgrammingCode" sheetId="30" r:id="rId10"/>
+    <sheet name="OutputCodeParameters" sheetId="34" r:id="rId11"/>
+    <sheet name="OutputDocumentRefs" sheetId="31" r:id="rId12"/>
+    <sheet name="DataSubsets" sheetId="6" r:id="rId13"/>
+    <sheet name="AnalysisSets" sheetId="1" r:id="rId14"/>
+    <sheet name="AnalysisGroupings" sheetId="2" r:id="rId15"/>
+    <sheet name="Analyses" sheetId="3" r:id="rId16"/>
+    <sheet name="AnalysisProgrammingCode" sheetId="27" r:id="rId17"/>
+    <sheet name="AnalysisCodeParameters" sheetId="32" r:id="rId18"/>
+    <sheet name="AnalysisDocumentRefs" sheetId="24" r:id="rId19"/>
+    <sheet name="AnalysisMethods" sheetId="4" r:id="rId20"/>
+    <sheet name="AnalysisMethodCodeTemplate" sheetId="23" r:id="rId21"/>
+    <sheet name="AnalysisMethodCodeParameters" sheetId="33" r:id="rId22"/>
+    <sheet name="AnalysisMethodDocumentRefs" sheetId="26" r:id="rId23"/>
+    <sheet name="AnalysisResults" sheetId="7" r:id="rId24"/>
+    <sheet name="TerminologyExtensions" sheetId="21" r:id="rId25"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Analyses!$A$1:$U$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">AnalysisDocumentRefs!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AnalysisMethods!$A$1:$P$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">AnalysisProgrammingCode!$A$1:$D$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">AnalysisResults!$A$1:$U$2</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">DataSubsets!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Displays!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">OutputDocumentRefs!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Analyses!$A$1:$W$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">AnalysisDocumentRefs!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">AnalysisMethods!$A$1:$R$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">AnalysisProgrammingCode!$A$1:$D$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">AnalysisResults!$A$1:$U$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">DataSubsets!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Displays!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">OutputDocumentRefs!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">OutputFiles!$A$1:$F$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029" calcMode="manual" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -138,7 +140,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -160,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="120">
   <si>
     <t>id</t>
   </si>
@@ -216,9 +218,6 @@
     <t>group_condition_value</t>
   </si>
   <si>
-    <t>grouping_type</t>
-  </si>
-  <si>
     <t>version</t>
   </si>
   <si>
@@ -261,12 +260,6 @@
     <t>displayTitle</t>
   </si>
   <si>
-    <t>fileSpecification_file_name</t>
-  </si>
-  <si>
-    <t>fileSpecification_file_location</t>
-  </si>
-  <si>
     <t>displaySection_sectionType</t>
   </si>
   <si>
@@ -279,9 +272,6 @@
     <t>display1_id</t>
   </si>
   <si>
-    <t>fileSpecification_file_fileType(s)</t>
-  </si>
-  <si>
     <t>analysisSet_label</t>
   </si>
   <si>
@@ -315,12 +305,6 @@
     <t>groupingId3</t>
   </si>
   <si>
-    <t>analysisId</t>
-  </si>
-  <si>
-    <t>outputId</t>
-  </si>
-  <si>
     <t>resultGroup1_groupingId</t>
   </si>
   <si>
@@ -484,13 +468,67 @@
   </si>
   <si>
     <t>operation_referencedResultRelationships2_description</t>
+  </si>
+  <si>
+    <t>display2_id</t>
+  </si>
+  <si>
+    <t>listItem_level</t>
+  </si>
+  <si>
+    <t>listItem_name</t>
+  </si>
+  <si>
+    <t>listItem_description</t>
+  </si>
+  <si>
+    <t>listItem_label</t>
+  </si>
+  <si>
+    <t>listItem_order</t>
+  </si>
+  <si>
+    <t>listItem_analysisId</t>
+  </si>
+  <si>
+    <t>listItem_outputId</t>
+  </si>
+  <si>
+    <t>fileType</t>
+  </si>
+  <si>
+    <t>operation_description</t>
+  </si>
+  <si>
+    <t>parameter_label</t>
+  </si>
+  <si>
+    <t>groupingDataset</t>
+  </si>
+  <si>
+    <t>group_name</t>
+  </si>
+  <si>
+    <t>group_description</t>
+  </si>
+  <si>
+    <t>operation_referencedResultRelationships1_analysisId</t>
+  </si>
+  <si>
+    <t>operation_referencedResultRelationships2_analysisId</t>
+  </si>
+  <si>
+    <t>compoundExpression_subClauseId</t>
+  </si>
+  <si>
+    <t>group_compoundExpression_subClauseId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -517,6 +555,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -545,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -559,6 +605,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,9 +624,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -617,7 +664,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -723,7 +770,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -865,7 +912,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -873,24 +920,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5945FE14-B7CD-4113-88D6-525465F971DD}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="21.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.86328125" customWidth="1"/>
+    <col min="5" max="5" width="24.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -899,8 +954,46 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF4F43AB-08A9-4D5D-BC36-392099289A62}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="34.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{AFBCF27C-42FB-4934-B668-A0446B0CFA1C}">
+      <formula1>"Code,DocumentRef"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB264D80-6970-406C-8A9F-6A5C48FD0FE0}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -909,21 +1002,25 @@
     <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.19921875" customWidth="1"/>
+    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -931,7 +1028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44891FB9-A2CE-4D40-A988-A4A68CEC1B08}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -949,22 +1046,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -982,107 +1079,130 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{317E84A7-ED57-45F7-86AC-94BF9578A26E}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="23.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.796875" customWidth="1"/>
+    <col min="3" max="3" width="28.19921875" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="4.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.1328125" customWidth="1"/>
+    <col min="9" max="9" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.53125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1" xr:uid="{317E84A7-ED57-45F7-86AC-94BF9578A26E}"/>
+  <autoFilter ref="A1:L1" xr:uid="{317E84A7-ED57-45F7-86AC-94BF9578A26E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2057B85-CDD2-49FA-961B-BE66955E248E}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="5.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.3984375" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" customWidth="1"/>
+    <col min="6" max="6" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.265625" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1092,79 +1212,90 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD49E34F-52D6-4F1E-B1C2-4599C0323EA6}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.796875" customWidth="1"/>
-    <col min="11" max="11" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.06640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.19921875" customWidth="1"/>
+    <col min="6" max="6" width="15.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.53125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="22.53125" customWidth="1"/>
+    <col min="11" max="11" width="22.9296875" customWidth="1"/>
+    <col min="12" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="18.1328125" customWidth="1"/>
+    <col min="16" max="16" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.06640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A2" t="str">
-        <f t="shared" ref="A2" si="0">IF(K2="ADSL","Subject","Data")</f>
-        <v>Data</v>
       </c>
     </row>
   </sheetData>
@@ -1174,10 +1305,10 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB53023-B5E5-496E-A786-48C47411B817}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1186,99 +1317,107 @@
     <col min="1" max="1" width="35.1328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="94.46484375" customWidth="1"/>
-    <col min="4" max="4" width="27.73046875" customWidth="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.86328125" customWidth="1"/>
+    <col min="5" max="5" width="33.3984375" customWidth="1"/>
+    <col min="6" max="6" width="27.73046875" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.53125" customWidth="1"/>
+    <col min="12" max="12" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.46484375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.19921875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.19921875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.86328125" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" customWidth="1"/>
-    <col min="20" max="20" width="28.3984375" customWidth="1"/>
-    <col min="21" max="21" width="16.265625" customWidth="1"/>
+    <col min="14" max="14" width="20.53125" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.46484375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.86328125" customWidth="1"/>
+    <col min="21" max="21" width="20.6640625" customWidth="1"/>
+    <col min="22" max="22" width="28.3984375" customWidth="1"/>
+    <col min="23" max="23" width="16.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>48</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U1" xr:uid="{4AB53023-B5E5-496E-A786-48C47411B817}"/>
+  <autoFilter ref="A1:W1" xr:uid="{4AB53023-B5E5-496E-A786-48C47411B817}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7330FD-BC60-4063-AD51-1ADCE1E2B7CF}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -1294,16 +1433,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -1336,9 +1475,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCEEFCB-4AF8-4DF4-9DD6-EB21C9658A74}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1347,21 +1486,25 @@
     <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>91</v>
+        <v>112</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1369,7 +1512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E9726D-99E8-44E0-8F39-A719318C5D2B}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1387,22 +1530,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1412,10 +1555,46 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63425975-7444-4301-ABB6-796B2115B6F2}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="21.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="34.06640625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="43.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC97203C-D8B1-4020-B955-08EA542F4944}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1423,76 +1602,86 @@
   <cols>
     <col min="1" max="1" width="26.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="85.6640625" customWidth="1"/>
+    <col min="3" max="3" width="85.6640625" customWidth="1"/>
+    <col min="4" max="4" width="35.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="34.796875" customWidth="1"/>
     <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="33.53125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.53125" customWidth="1"/>
-    <col min="12" max="13" width="33.53125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.46484375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.73046875" customWidth="1"/>
-    <col min="16" max="17" width="26.9296875" customWidth="1"/>
+    <col min="8" max="8" width="14.9296875" customWidth="1"/>
+    <col min="9" max="9" width="23" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="33.53125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="33.53125" customWidth="1"/>
+    <col min="13" max="15" width="33.53125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="38.46484375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.73046875" customWidth="1"/>
+    <col min="18" max="20" width="26.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>107</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L19">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M19">
     <sortCondition ref="A2:A19"/>
     <sortCondition ref="G2:G19"/>
   </sortState>
@@ -1500,36 +1689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63425975-7444-4301-ABB6-796B2115B6F2}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="21.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.06640625" customWidth="1"/>
-    <col min="3" max="3" width="43.86328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5A7EA2-5BB8-48A0-AE19-CC45569B1AA0}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -1545,16 +1705,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
@@ -1573,9 +1733,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06F5578B-A7DE-401B-B867-DFECFDE9AF0A}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1584,25 +1744,29 @@
     <col min="1" max="1" width="26.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.06640625" customWidth="1"/>
+    <col min="5" max="5" width="33.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1611,7 +1775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26572EB2-03E0-4576-A1FD-245E2B761D42}">
   <dimension ref="A1:F1"/>
   <sheetViews>
@@ -1629,22 +1793,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1661,7 +1825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BB806F-07BC-44FD-839E-73D40D8773BC}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:U19"/>
@@ -1696,73 +1860,73 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B2" s="3" t="e" cm="1">
-        <f t="array" ref="B2">_xlfn._xlws.FILTER(AnalysisSets!B:B,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!G:G,Analyses!A:A=AnalysisResults!A2,""),"")</f>
+        <f t="array" ref="B2">_xlfn._xlws.FILTER(AnalysisSets!D:D,AnalysisSets!A:A=_xlfn._xlws.FILTER(Analyses!I:I,Analyses!A:A=AnalysisResults!A2,""),"")</f>
         <v>#N/A</v>
       </c>
       <c r="D2" s="3" cm="1">
-        <f t="array" ref="D2">_xlfn.UNIQUE(_xlfn._xlws.FILTER(AnalysisMethods!$C$2:$C$19,AnalysisMethods!$A$2:$A$19=AnalysisResults!C2,""))</f>
+        <f t="array" ref="D2">_xlfn.UNIQUE(_xlfn._xlws.FILTER(AnalysisMethods!$D$2:$D$19,AnalysisMethods!$A$2:$A$19=AnalysisResults!C2,""))</f>
         <v>0</v>
       </c>
       <c r="F2" s="3" cm="1">
@@ -1770,19 +1934,19 @@
         <v>0</v>
       </c>
       <c r="G2" s="3" cm="1">
-        <f t="array" ref="G2:G19">_xlfn._xlws.FILTER(AnalysisMethods!$I$2:$I$19,AnalysisMethods!$E$2:$E$19=AnalysisResults!E2,"")</f>
+        <f t="array" ref="G2:G19">_xlfn._xlws.FILTER(AnalysisMethods!$J$2:$J$19,AnalysisMethods!$E$2:$E$19=AnalysisResults!E2,"")</f>
         <v>0</v>
       </c>
       <c r="J2" s="3" t="str" cm="1">
-        <f t="array" ref="J2">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$2,(AnalysisGroupings!$F$2:$F$2=AnalysisResults!I2)*LEN(I2)&gt;0,"")</f>
+        <f t="array" ref="J2">_xlfn._xlws.FILTER(AnalysisGroupings!$K$2:$K$2,(AnalysisGroupings!$H$2:$H$2=AnalysisResults!I2)*LEN(I2)&gt;0,"")</f>
         <v/>
       </c>
       <c r="N2" s="3" t="str" cm="1">
-        <f t="array" ref="N2">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$2,(AnalysisGroupings!$F$2:$F$2=AnalysisResults!M2)*LEN(M2)&gt;0,"")</f>
+        <f t="array" ref="N2">_xlfn._xlws.FILTER(AnalysisGroupings!$K$2:$K$2,(AnalysisGroupings!$H$2:$H$2=AnalysisResults!M2)*LEN(M2)&gt;0,"")</f>
         <v/>
       </c>
       <c r="R2" s="3" t="str" cm="1">
-        <f t="array" ref="R2">_xlfn._xlws.FILTER(AnalysisGroupings!$G$2:$G$2,(AnalysisGroupings!$F$2:$F$2=AnalysisResults!Q2)*LEN(Q2)&gt;0,"")</f>
+        <f t="array" ref="R2">_xlfn._xlws.FILTER(AnalysisGroupings!$K$2:$K$2,(AnalysisGroupings!$H$2:$H$2=AnalysisResults!Q2)*LEN(Q2)&gt;0,"")</f>
         <v/>
       </c>
     </row>
@@ -1935,7 +2099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C6F21E-B0BD-4A7C-9873-05E64DE79965}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1951,16 +2115,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1996,13 +2160,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2014,32 +2178,52 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04E4817-59BC-4505-A834-22FE96EF578C}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="85.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.06640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>104</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2050,32 +2234,53 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78005A0C-8AA5-4998-8A42-428CFBB35FD9}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="80.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.06640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" customWidth="1"/>
+    <col min="6" max="6" width="45.3984375" customWidth="1"/>
+    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="8" max="8" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>104</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -2092,27 +2297,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.53125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A23" xr:uid="{6F5061BD-D187-4B34-B453-5F022522F44D}">
-      <formula1>"Title,Footnote,Abbreviation,Legend,Rowlabel Header"</formula1>
+      <formula1>"Header,Title,Rowlabel Header,Legend,Abbreviation,Footnote,Footer"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2132,15 +2337,17 @@
     <col min="1" max="1" width="11.265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="78.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.59765625" customWidth="1"/>
-    <col min="6" max="6" width="35.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.46484375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.9296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.19921875" customWidth="1"/>
+    <col min="5" max="5" width="27.53125" customWidth="1"/>
+    <col min="6" max="6" width="40.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1328125" customWidth="1"/>
+    <col min="8" max="8" width="18.59765625" customWidth="1"/>
+    <col min="9" max="9" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
@@ -2148,25 +2355,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2175,88 +2382,102 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE8E678-724A-495B-ACBB-35EFE50A29D5}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.46484375" customWidth="1"/>
+    <col min="2" max="2" width="26.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.46484375" customWidth="1"/>
+    <col min="5" max="5" width="28.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{0BE8E678-724A-495B-ACBB-35EFE50A29D5}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3266631C-B97C-414A-AC8B-8A56E4E40917}">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.06640625" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.6640625" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="27.06640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="54.53125" customWidth="1"/>
+    <col min="2" max="4" width="13.06640625" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79.6640625" customWidth="1"/>
+    <col min="7" max="7" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" customWidth="1"/>
+    <col min="9" max="9" width="27.06640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>37</v>
+        <v>93</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{3266631C-B97C-414A-AC8B-8A56E4E40917}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF4F43AB-08A9-4D5D-BC36-392099289A62}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="34.53125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-  </sheetData>
+  <autoFilter ref="A1:J1" xr:uid="{3266631C-B97C-414A-AC8B-8A56E4E40917}"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{AFBCF27C-42FB-4934-B668-A0446B0CFA1C}">
-      <formula1>"Code,DocumentRef"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{6886E7E9-749C-4246-A4F8-34848082C1DA}">
+      <formula1>"Header,Title,Rowlabel Header,Legend,Abbreviation,Footnote,Footer"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Utility bug fixes (#224, #227, #228, #229)
</commit_message>
<xml_diff>
--- a/utilities/python/ARS Template.xlsx
+++ b/utilities/python/ARS Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDISC\ars\analysis-results-standard\utilities\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDB610B-F10C-4889-AC61-E0EF2010FD37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC97DA0-3134-4583-A0AF-E4B9C983DED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="127" yWindow="0" windowWidth="21601" windowHeight="11400" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
+    <workbookView xWindow="4665" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{0614A9B4-62F8-4E97-B269-DF8F18CCF706}"/>
   </bookViews>
   <sheets>
     <sheet name="ReportingEvent" sheetId="19" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">OutputDocumentRefs!$A$1:$F$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">OutputFiles!$A$1:$F$1</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcMode="manual" refMode="R1C1"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="120">
   <si>
     <t>id</t>
   </si>
@@ -2101,35 +2101,38 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C6F21E-B0BD-4A7C-9873-05E64DE79965}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.3984375" customWidth="1"/>
-    <col min="4" max="4" width="52.796875" customWidth="1"/>
+    <col min="2" max="2" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.3984375" customWidth="1"/>
+    <col min="5" max="5" width="52.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A24" xr:uid="{0A7C3BAC-D424-43D3-9B4E-1A4E4E37AE75}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B24" xr:uid="{0A7C3BAC-D424-43D3-9B4E-1A4E4E37AE75}">
       <formula1>"AnalysisReason,AnalysisPurpose,OperationRole,OutputFileType"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>